<commit_message>
Second commit final exam
</commit_message>
<xml_diff>
--- a/Final_computerTools.xlsx
+++ b/Final_computerTools.xlsx
@@ -5,27 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\collage\computer-tools\final_exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B066FD4A-CA5D-4F5E-9F66-E5481592D48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA23AE5B-3A52-48B2-85E6-C6999FCB715E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BE5C0321-A9A6-485E-94A6-185A66B45C65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{BE5C0321-A9A6-485E-94A6-185A66B45C65}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="3" r:id="rId1"/>
     <sheet name="2" sheetId="1" r:id="rId2"/>
     <sheet name="3" sheetId="2" r:id="rId3"/>
-    <sheet name="5" sheetId="4" r:id="rId4"/>
-    <sheet name="6" sheetId="5" r:id="rId5"/>
-    <sheet name="7" sheetId="6" r:id="rId6"/>
-    <sheet name="8" sheetId="7" r:id="rId7"/>
-    <sheet name="9" sheetId="8" r:id="rId8"/>
-    <sheet name="10" sheetId="9" r:id="rId9"/>
-    <sheet name="11" sheetId="10" r:id="rId10"/>
-    <sheet name="12" sheetId="11" r:id="rId11"/>
-    <sheet name="Question 3-1" sheetId="12" r:id="rId12"/>
-    <sheet name="Question 3 - 2" sheetId="14" r:id="rId13"/>
+    <sheet name="4" sheetId="15" r:id="rId4"/>
+    <sheet name="5" sheetId="4" r:id="rId5"/>
+    <sheet name="6" sheetId="5" r:id="rId6"/>
+    <sheet name="7" sheetId="6" r:id="rId7"/>
+    <sheet name="8" sheetId="7" r:id="rId8"/>
+    <sheet name="9" sheetId="8" r:id="rId9"/>
+    <sheet name="10" sheetId="9" r:id="rId10"/>
+    <sheet name="11" sheetId="10" r:id="rId11"/>
+    <sheet name="12" sheetId="11" r:id="rId12"/>
+    <sheet name="Question 3-1" sheetId="12" r:id="rId13"/>
+    <sheet name="Question 3 - 2" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1'!$B$1:$D$13</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="37">
   <si>
     <t>OrderDate</t>
   </si>
@@ -177,6 +178,12 @@
   </si>
   <si>
     <t>Unit price less than 150</t>
+  </si>
+  <si>
+    <t>Statement</t>
+  </si>
+  <si>
+    <t>Total price Carrot for west</t>
   </si>
 </sst>
 </file>
@@ -3823,6 +3830,395 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9315D44-DCA7-4A85-9D95-58AE8DDB582D}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>43831</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5">
+        <v>33</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1.77</v>
+      </c>
+      <c r="H2" s="5">
+        <f>F2*G2</f>
+        <v>58.410000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>43834</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5">
+        <v>87</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3.49</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H13" si="0">F3*G3</f>
+        <v>303.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>43837</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5">
+        <v>58</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>108.46000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>43840</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5">
+        <v>82</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="0"/>
+        <v>153.34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>43843</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5">
+        <v>38</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="0"/>
+        <v>82.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>43846</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5">
+        <v>54</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1.77</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="0"/>
+        <v>95.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>43849</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5">
+        <v>149</v>
+      </c>
+      <c r="G8" s="5">
+        <v>3.49</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>520.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>43852</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="5">
+        <v>51</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1.77</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="0"/>
+        <v>90.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>43855</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5">
+        <v>100</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1.77</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="0"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>43858</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5">
+        <v>28</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1.35</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="0"/>
+        <v>37.800000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>43861</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="5">
+        <v>36</v>
+      </c>
+      <c r="G12" s="5">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="0"/>
+        <v>78.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>43864</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="5">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1.87</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="0"/>
+        <v>57.970000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16">
+        <f>COUNTIF(D2:D13,"Crackers")</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97CE1AE-3422-4729-859C-0DADF1DA67D6}">
   <dimension ref="A1:I20"/>
   <sheetViews>
@@ -4229,7 +4625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B067592-D0A5-4406-A5CE-3DFADEB361CE}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -4619,7 +5015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541AD07B-7BCF-4B49-90DE-CEE2240B1E5D}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -4996,7 +5392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C2D46-CA5A-4947-8741-E19A532DDEED}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -5750,8 +6146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB65B4AB-0636-4C75-B394-787C2701BB15}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6147,6 +6543,396 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CF10C9-10BB-4298-8272-ED588A4F4DAF}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>43831</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="8">
+        <v>33</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1.77</v>
+      </c>
+      <c r="H2" s="8">
+        <f>F2*G2</f>
+        <v>58.410000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>43834</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8">
+        <v>87</v>
+      </c>
+      <c r="G3" s="8">
+        <v>3.49</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H13" si="0">F3*G3</f>
+        <v>303.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>43837</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="8">
+        <v>58</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1.87</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="0"/>
+        <v>108.46000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>43840</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8">
+        <v>82</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1.87</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" si="0"/>
+        <v>153.34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>43843</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="8">
+        <v>38</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="0"/>
+        <v>82.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>43846</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="8">
+        <v>54</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1.77</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>95.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>43849</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="8">
+        <v>149</v>
+      </c>
+      <c r="G8" s="8">
+        <v>3.49</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="0"/>
+        <v>520.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>43852</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8">
+        <v>51</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1.77</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="0"/>
+        <v>90.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>43855</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="8">
+        <v>100</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1.77</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="0"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>43858</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8">
+        <v>28</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1.35</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="0"/>
+        <v>37.800000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>43861</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8">
+        <v>36</v>
+      </c>
+      <c r="G12" s="8">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="0"/>
+        <v>78.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>43864</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="8">
+        <v>31</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1.87</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="0"/>
+        <v>57.970000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="2">
+        <f>SUMIFS(H2:H13,B2:B13,"West",E2:E13,"Carrot")</f>
+        <v>90.27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0952169D-0F31-4B6E-8231-FF9FB377A07D}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -6534,7 +7320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A4001D-615C-4441-8444-1EE3A55B0C3C}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -6926,7 +7712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDD5144-E254-45A4-BA77-A5963DFE73D8}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -7311,7 +8097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BE52D5-B41D-47F1-9037-3EA394BC8E68}">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -7694,7 +8480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BD5C8F-E0FA-46DF-9EED-908E1D4317FB}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -8080,393 +8866,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9315D44-DCA7-4A85-9D95-58AE8DDB582D}">
-  <dimension ref="A1:H16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>43831</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="5">
-        <v>33</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1.77</v>
-      </c>
-      <c r="H2" s="5">
-        <f>F2*G2</f>
-        <v>58.410000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>43834</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="5">
-        <v>87</v>
-      </c>
-      <c r="G3" s="5">
-        <v>3.49</v>
-      </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H13" si="0">F3*G3</f>
-        <v>303.63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>43837</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="5">
-        <v>58</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1.87</v>
-      </c>
-      <c r="H4" s="5">
-        <f t="shared" si="0"/>
-        <v>108.46000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>43840</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5">
-        <v>82</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1.87</v>
-      </c>
-      <c r="H5" s="5">
-        <f t="shared" si="0"/>
-        <v>153.34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>43843</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="5">
-        <v>38</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="H6" s="5">
-        <f t="shared" si="0"/>
-        <v>82.84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>43846</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="5">
-        <v>54</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1.77</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" si="0"/>
-        <v>95.58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>43849</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="5">
-        <v>149</v>
-      </c>
-      <c r="G8" s="5">
-        <v>3.49</v>
-      </c>
-      <c r="H8" s="5">
-        <f t="shared" si="0"/>
-        <v>520.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>43852</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="5">
-        <v>51</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1.77</v>
-      </c>
-      <c r="H9" s="5">
-        <f t="shared" si="0"/>
-        <v>90.27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>43855</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="5">
-        <v>100</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1.77</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>43858</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="5">
-        <v>28</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1.35</v>
-      </c>
-      <c r="H11" s="5">
-        <f t="shared" si="0"/>
-        <v>37.800000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>43861</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="5">
-        <v>36</v>
-      </c>
-      <c r="G12" s="5">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="H12" s="5">
-        <f t="shared" si="0"/>
-        <v>78.48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>43864</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="5">
-        <v>31</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1.87</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="0"/>
-        <v>57.970000000000006</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16">
-        <f>COUNTIF(D2:D13,"Crackers")</f>
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>